<commit_message>
Added a keyboard scanner routine to the client. Doesn't do n-rollover yet.
</commit_message>
<xml_diff>
--- a/docs/keyboard.xlsx
+++ b/docs/keyboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF59CAA-F96B-40D8-9754-303839A272F7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7BD4DD-2501-4605-90DC-47AD5E41B595}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{4BA65098-C843-4DE0-8A66-918AFB495216}"/>
   </bookViews>
@@ -133,7 +133,7 @@
     <t>Caps Shift</t>
   </si>
   <si>
-    <t xml:space="preserve">  ;  Row   Bit0   Bit1   Bit2   Bit3   Bit4  Index  Row      Modifier</t>
+    <t xml:space="preserve">  ; Mark   Row   Bit0   Bit1   Bit2   Bit3   Bit4  Index  Row      Modifier</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\B\i\t0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,17 +182,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -250,13 +257,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -581,7 +591,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
@@ -596,11 +606,11 @@
     <col min="10" max="14" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="98.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -643,10 +653,10 @@
       <c r="N1" s="7">
         <v>4</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>12</v>
       </c>
       <c r="Q1" s="13" t="s">
@@ -713,9 +723,9 @@
         <f>"$" &amp; VLOOKUP(D2, Rows!$J:$K, 2, FALSE)</f>
         <v>$7F</v>
       </c>
-      <c r="Q2" s="12" t="str">
-        <f>"  db " &amp; P2 &amp; ",  " &amp; J2 &amp; ",  " &amp; K2 &amp; ",  " &amp; L2 &amp; ",  " &amp; M2 &amp; ",  " &amp; N2 &amp; "  ;  " &amp; RIGHT(" " &amp; A2, 2) &amp; "  " &amp; LEFT(MID(D2, 3, 99) &amp; "      ", 7) &amp; "  " &amp; O2</f>
-        <v xml:space="preserve">  db $7F,   $20,  None,   $6D,   $6E,   $62  ;   0  BNMSsSp  None</v>
+      <c r="Q2" s="14" t="str">
+        <f>"  db $FF,  " &amp; P2 &amp; ",  " &amp; J2 &amp; ",  " &amp; K2 &amp; ",  " &amp; L2 &amp; ",  " &amp; M2 &amp; ",  " &amp; N2 &amp; "  ;  " &amp; RIGHT(" " &amp; A2, 2) &amp; "  " &amp; LEFT(MID(D2, 3, 99) &amp; "      ", 7) &amp; "  " &amp; O2</f>
+        <v xml:space="preserve">  db $FF,  $7F,   $20,  None,   $6D,   $6E,   $62  ;   0  BNMSsSp  None</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -779,9 +789,9 @@
         <f>"$" &amp; VLOOKUP(D3, Rows!$J:$K, 2, FALSE)</f>
         <v>$BF</v>
       </c>
-      <c r="Q3" s="12" t="str">
-        <f t="shared" ref="Q3:Q25" si="0">"  db " &amp; P3 &amp; ",  " &amp; J3 &amp; ",  " &amp; K3 &amp; ",  " &amp; L3 &amp; ",  " &amp; M3 &amp; ",  " &amp; N3 &amp; "  ;  " &amp; RIGHT(" " &amp; A3, 2) &amp; "  " &amp; LEFT(MID(D3, 3, 99) &amp; "      ", 7) &amp; "  " &amp; O3</f>
-        <v xml:space="preserve">  db $BF,   $5F,   $6C,   $6B,   $6A,   $68  ;   1  HJKLEn   None</v>
+      <c r="Q3" s="14" t="str">
+        <f t="shared" ref="Q3:Q25" si="0">"  db $FF,  " &amp; P3 &amp; ",  " &amp; J3 &amp; ",  " &amp; K3 &amp; ",  " &amp; L3 &amp; ",  " &amp; M3 &amp; ",  " &amp; N3 &amp; "  ;  " &amp; RIGHT(" " &amp; A3, 2) &amp; "  " &amp; LEFT(MID(D3, 3, 99) &amp; "      ", 7) &amp; "  " &amp; O3</f>
+        <v xml:space="preserve">  db $FF,  $BF,   $5F,   $6C,   $6B,   $6A,   $68  ;   1  HJKLEn   None</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -845,9 +855,9 @@
         <f>"$" &amp; VLOOKUP(D4, Rows!$J:$K, 2, FALSE)</f>
         <v>$DF</v>
       </c>
-      <c r="Q4" s="12" t="str">
+      <c r="Q4" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $DF,   $70,   $6F,   $69,   $75,   $79  ;   2  YUIOP    None</v>
+        <v xml:space="preserve">  db $FF,  $DF,   $70,   $6F,   $69,   $75,   $79  ;   2  YUIOP    None</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -911,9 +921,9 @@
         <f>"$" &amp; VLOOKUP(D5, Rows!$J:$K, 2, FALSE)</f>
         <v>$EF</v>
       </c>
-      <c r="Q5" s="12" t="str">
+      <c r="Q5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $EF,   $30,   $39,   $38,   $37,   $36  ;   3  67890    None</v>
+        <v xml:space="preserve">  db $FF,  $EF,   $30,   $39,   $38,   $37,   $36  ;   3  67890    None</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -977,9 +987,9 @@
         <f>"$" &amp; VLOOKUP(D6, Rows!$J:$K, 2, FALSE)</f>
         <v>$F7</v>
       </c>
-      <c r="Q6" s="12" t="str">
+      <c r="Q6" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $F7,   $31,   $32,   $33,   $34,   $35  ;   4  54321    None</v>
+        <v xml:space="preserve">  db $FF,  $F7,   $31,   $32,   $33,   $34,   $35  ;   4  54321    None</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1043,9 +1053,9 @@
         <f>"$" &amp; VLOOKUP(D7, Rows!$J:$K, 2, FALSE)</f>
         <v>$FB</v>
       </c>
-      <c r="Q7" s="12" t="str">
+      <c r="Q7" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FB,   $71,   $77,   $65,   $72,   $74  ;   5  TREWQ    None</v>
+        <v xml:space="preserve">  db $FF,  $FB,   $71,   $77,   $65,   $72,   $74  ;   5  TREWQ    None</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1109,9 +1119,9 @@
         <f>"$" &amp; VLOOKUP(D8, Rows!$J:$K, 2, FALSE)</f>
         <v>$FD</v>
       </c>
-      <c r="Q8" s="12" t="str">
+      <c r="Q8" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FD,   $61,   $73,   $64,   $66,   $67  ;   6  GFDSA    None</v>
+        <v xml:space="preserve">  db $FF,  $FD,   $61,   $73,   $64,   $66,   $67  ;   6  GFDSA    None</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1175,9 +1185,9 @@
         <f>"$" &amp; VLOOKUP(D9, Rows!$J:$K, 2, FALSE)</f>
         <v>$FE</v>
       </c>
-      <c r="Q9" s="12" t="str">
+      <c r="Q9" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FE,  None,   $7A,   $78,   $63,   $76  ;   7  VCXZCs   None</v>
+        <v xml:space="preserve">  db $FF,  $FE,  None,   $7A,   $78,   $63,   $76  ;   7  VCXZCs   None</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1241,9 +1251,9 @@
         <f>"$" &amp; VLOOKUP(D10, Rows!$J:$K, 2, FALSE)</f>
         <v>$7F</v>
       </c>
-      <c r="Q10" s="12" t="str">
+      <c r="Q10" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $7F,  None,  None,   $2E,   $2C,   $2A  ;   8  BNMSsSp  Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $7F,  None,  None,   $2E,   $2C,   $2A  ;   8  BNMSsSp  Symbol Shift</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1307,9 +1317,9 @@
         <f>"$" &amp; VLOOKUP(D11, Rows!$J:$K, 2, FALSE)</f>
         <v>$BF</v>
       </c>
-      <c r="Q11" s="12" t="str">
+      <c r="Q11" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $BF,  None,   $3D,  None,   $2B,  None  ;   9  HJKLEn   Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $BF,  None,   $3D,  None,   $2B,  None  ;   9  HJKLEn   Symbol Shift</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1373,9 +1383,9 @@
         <f>"$" &amp; VLOOKUP(D12, Rows!$J:$K, 2, FALSE)</f>
         <v>$DF</v>
       </c>
-      <c r="Q12" s="12" t="str">
+      <c r="Q12" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $DF,   $22,   $3B,  None,  None,  None  ;  10  YUIOP    Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $DF,   $22,   $3B,  None,  None,  None  ;  10  YUIOP    Symbol Shift</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1439,9 +1449,9 @@
         <f>"$" &amp; VLOOKUP(D13, Rows!$J:$K, 2, FALSE)</f>
         <v>$EF</v>
       </c>
-      <c r="Q13" s="12" t="str">
+      <c r="Q13" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $EF,  None,   $29,   $28,   $27,   $26  ;  11  67890    Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $EF,  None,   $29,   $28,   $27,   $26  ;  11  67890    Symbol Shift</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1505,9 +1515,9 @@
         <f>"$" &amp; VLOOKUP(D14, Rows!$J:$K, 2, FALSE)</f>
         <v>$F7</v>
       </c>
-      <c r="Q14" s="12" t="str">
+      <c r="Q14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $F7,   $21,   $40,  None,   $24,   $25  ;  12  54321    Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $F7,   $21,   $40,  None,   $24,   $25  ;  12  54321    Symbol Shift</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1571,9 +1581,9 @@
         <f>"$" &amp; VLOOKUP(D15, Rows!$J:$K, 2, FALSE)</f>
         <v>$FB</v>
       </c>
-      <c r="Q15" s="12" t="str">
+      <c r="Q15" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FB,  None,  None,  None,   $3C,   $3E  ;  13  TREWQ    Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $FB,  None,  None,  None,   $3C,   $3E  ;  13  TREWQ    Symbol Shift</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1637,9 +1647,9 @@
         <f>"$" &amp; VLOOKUP(D16, Rows!$J:$K, 2, FALSE)</f>
         <v>$FD</v>
       </c>
-      <c r="Q16" s="12" t="str">
+      <c r="Q16" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FD,  None,  None,  None,  None,  None  ;  14  GFDSA    Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $FD,  None,  None,  None,  None,  None  ;  14  GFDSA    Symbol Shift</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1703,9 +1713,9 @@
         <f>"$" &amp; VLOOKUP(D17, Rows!$J:$K, 2, FALSE)</f>
         <v>$FE</v>
       </c>
-      <c r="Q17" s="12" t="str">
+      <c r="Q17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FE,  None,   $3A,   $23,   $3F,   $2F  ;  15  VCXZCs   Symbol Shift</v>
+        <v xml:space="preserve">  db $FF,  $FE,  None,   $3A,   $23,   $3F,   $2F  ;  15  VCXZCs   Symbol Shift</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1769,9 +1779,9 @@
         <f>"$" &amp; VLOOKUP(D18, Rows!$J:$K, 2, FALSE)</f>
         <v>$7F</v>
       </c>
-      <c r="Q18" s="12" t="str">
+      <c r="Q18" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $7F,  None,  None,   $4D,   $4E,   $42  ;  16  BNMSsSp  Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $7F,  None,  None,   $4D,   $4E,   $42  ;  16  BNMSsSp  Caps Shift</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1835,9 +1845,9 @@
         <f>"$" &amp; VLOOKUP(D19, Rows!$J:$K, 2, FALSE)</f>
         <v>$BF</v>
       </c>
-      <c r="Q19" s="12" t="str">
+      <c r="Q19" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $BF,  None,   $4C,   $4B,   $4A,   $48  ;  17  HJKLEn   Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $BF,  None,   $4C,   $4B,   $4A,   $48  ;  17  HJKLEn   Caps Shift</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1901,9 +1911,9 @@
         <f>"$" &amp; VLOOKUP(D20, Rows!$J:$K, 2, FALSE)</f>
         <v>$DF</v>
       </c>
-      <c r="Q20" s="12" t="str">
+      <c r="Q20" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $DF,   $50,   $4F,   $49,   $55,   $59  ;  18  YUIOP    Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $DF,   $50,   $4F,   $49,   $55,   $59  ;  18  YUIOP    Caps Shift</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1922,7 +1932,7 @@
       </c>
       <c r="E21" s="10" t="str">
         <f>IF(ISNA(VLOOKUP($B21 &amp; $C21 &amp; E$1 &amp; $D21, Chars!$G:$I, 2, FALSE)), "", VLOOKUP($B21 &amp; $C21 &amp; E$1 &amp; $D21, Chars!$G:$I, 2, FALSE))</f>
-        <v/>
+        <v>DELETE</v>
       </c>
       <c r="F21" s="10" t="str">
         <f>IF(ISNA(VLOOKUP($B21 &amp; $C21 &amp; F$1 &amp; $D21, Chars!$G:$I, 2, FALSE)), "", VLOOKUP($B21 &amp; $C21 &amp; F$1 &amp; $D21, Chars!$G:$I, 2, FALSE))</f>
@@ -1942,7 +1952,7 @@
       </c>
       <c r="J21" s="10" t="str">
         <f>IF(ISNA(VLOOKUP($B21 &amp; $C21 &amp; J$1 &amp; $D21, Chars!$G:$I, 3, FALSE)), "None", " " &amp; VLOOKUP($B21 &amp; $C21 &amp; J$1 &amp; $D21, Chars!$G:$I, 3, FALSE))</f>
-        <v>None</v>
+        <v xml:space="preserve"> $7F</v>
       </c>
       <c r="K21" s="10" t="str">
         <f>IF(ISNA(VLOOKUP($B21 &amp; $C21 &amp; K$1 &amp; $D21, Chars!$G:$I, 3, FALSE)), "None", " " &amp; VLOOKUP($B21 &amp; $C21 &amp; K$1 &amp; $D21, Chars!$G:$I, 3, FALSE))</f>
@@ -1967,9 +1977,9 @@
         <f>"$" &amp; VLOOKUP(D21, Rows!$J:$K, 2, FALSE)</f>
         <v>$EF</v>
       </c>
-      <c r="Q21" s="12" t="str">
+      <c r="Q21" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $EF,  None,  None,  None,  None,  None  ;  19  67890    Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $EF,   $7F,  None,  None,  None,  None  ;  19  67890    Caps Shift</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2033,9 +2043,9 @@
         <f>"$" &amp; VLOOKUP(D22, Rows!$J:$K, 2, FALSE)</f>
         <v>$F7</v>
       </c>
-      <c r="Q22" s="12" t="str">
+      <c r="Q22" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $F7,  None,  None,  None,  None,  None  ;  20  54321    Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $F7,  None,  None,  None,  None,  None  ;  20  54321    Caps Shift</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2099,9 +2109,9 @@
         <f>"$" &amp; VLOOKUP(D23, Rows!$J:$K, 2, FALSE)</f>
         <v>$FB</v>
       </c>
-      <c r="Q23" s="12" t="str">
+      <c r="Q23" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FB,   $51,   $57,   $45,   $52,   $54  ;  21  TREWQ    Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $FB,   $51,   $57,   $45,   $52,   $54  ;  21  TREWQ    Caps Shift</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2165,9 +2175,9 @@
         <f>"$" &amp; VLOOKUP(D24, Rows!$J:$K, 2, FALSE)</f>
         <v>$FD</v>
       </c>
-      <c r="Q24" s="12" t="str">
+      <c r="Q24" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FD,   $41,   $53,   $44,   $46,   $47  ;  22  GFDSA    Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $FD,   $41,   $53,   $44,   $46,   $47  ;  22  GFDSA    Caps Shift</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2231,13 +2241,14 @@
         <f>"$" &amp; VLOOKUP(D25, Rows!$J:$K, 2, FALSE)</f>
         <v>$FE</v>
       </c>
-      <c r="Q25" s="12" t="str">
+      <c r="Q25" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  db $FE,  None,   $5A,   $58,   $43,   $56  ;  23  VCXZCs   Caps Shift</v>
+        <v xml:space="preserve">  db $FF,  $FE,  None,   $5A,   $58,   $43,   $56  ;  23  VCXZCs   Caps Shift</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -2246,8 +2257,8 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5917,7 +5928,7 @@
         <v>123</v>
       </c>
       <c r="G125" s="3" t="str">
-        <f t="shared" ref="G67:G129" si="14">F125&amp;C125</f>
+        <f t="shared" ref="G125:G129" si="14">F125&amp;C125</f>
         <v/>
       </c>
       <c r="H125" s="8" t="str">
@@ -6004,15 +6015,15 @@
         <v>0</v>
       </c>
       <c r="G129" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v>0K_67890</v>
+        <f t="shared" ref="G129" si="16">D129 &amp; E129 &amp; F129 &amp; C129</f>
+        <v>100K_67890</v>
       </c>
       <c r="H129" s="8" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="H129" si="17">B129&amp;""</f>
         <v>DELETE</v>
       </c>
       <c r="I129" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="I129" si="18">IF(ISBLANK(C129), "", "$" &amp; DEC2HEX(A129, 2))</f>
         <v>$7F</v>
       </c>
     </row>

</xml_diff>